<commit_message>
Added pattern fill for negative values
</commit_message>
<xml_diff>
--- a/documents/Published/Ring Chart/RingChartbyMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Ring Chart/RingChartbyMAQSoftwareChecklist.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Power BI\RingChart\17-10-17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RajveerC\Source\Repos\PowerBI-visuals\documents\Published\Ring Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C844181-A0C6-483F-B5FB-AA7A0A255B24}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15285" windowHeight="5310" xr2:uid="{298230A1-4D6D-45FE-9FCF-FFB948C6A0D6}"/>
   </bookViews>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="129">
   <si>
     <r>
       <t>#</t>
@@ -525,6 +526,21 @@
   </si>
   <si>
     <t>Secondary measure summary value should display value in 'Thousands' and with 2 decimal places</t>
+  </si>
+  <si>
+    <t>Negative Value</t>
+  </si>
+  <si>
+    <t>Check whether chart is ploting for negative values</t>
+  </si>
+  <si>
+    <t>1. Select value column with negative data to 'Primary Measure' input field
+2. Go to formatting pane.
+3. Turn on Pattern fill toggle.</t>
+  </si>
+  <si>
+    <t>Plot should render for negative values also and data labels should also appear for the respective arc.
+Arc for negative values are filled in line pattern.</t>
   </si>
 </sst>
 </file>
@@ -631,22 +647,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -962,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5BD6B43-E3C6-4B92-AF1B-22928F3D0975}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,7 +993,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -991,7 +1007,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1005,8 +1021,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="15" t="s">
         <v>37</v>
       </c>
       <c r="C3" t="s">
@@ -1017,8 +1033,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="15"/>
       <c r="C4" t="s">
         <v>38</v>
       </c>
@@ -1027,7 +1043,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1041,7 +1057,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="5" t="s">
         <v>44</v>
       </c>
@@ -1053,7 +1069,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1067,7 +1083,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="5" t="s">
         <v>51</v>
       </c>
@@ -1079,7 +1095,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="5" t="s">
         <v>54</v>
       </c>
@@ -1091,7 +1107,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="5" t="s">
         <v>57</v>
       </c>
@@ -1103,7 +1119,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="5" t="s">
         <v>60</v>
       </c>
@@ -1129,7 +1145,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>67</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1143,7 +1159,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5" t="s">
         <v>73</v>
       </c>
@@ -1155,7 +1171,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5" t="s">
         <v>72</v>
       </c>
@@ -1167,7 +1183,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="13" t="s">
         <v>76</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -1181,7 +1197,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5" t="s">
         <v>81</v>
       </c>
@@ -1193,7 +1209,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5" t="s">
         <v>85</v>
       </c>
@@ -1205,7 +1221,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>84</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -1219,7 +1235,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="5" t="s">
         <v>85</v>
       </c>
@@ -1231,7 +1247,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="13" t="s">
         <v>90</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -1245,7 +1261,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="5" t="s">
         <v>93</v>
       </c>
@@ -1257,7 +1273,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="5" t="s">
         <v>96</v>
       </c>
@@ -1269,7 +1285,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -1283,7 +1299,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="5" t="s">
         <v>102</v>
       </c>
@@ -1295,7 +1311,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="5" t="s">
         <v>105</v>
       </c>
@@ -1307,7 +1323,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>108</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -1321,7 +1337,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="5" t="s">
         <v>102</v>
       </c>
@@ -1333,7 +1349,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="5" t="s">
         <v>105</v>
       </c>
@@ -1345,7 +1361,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="11" t="s">
         <v>115</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1359,7 +1375,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="11" t="s">
         <v>118</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -1372,18 +1388,32 @@
         <v>121</v>
       </c>
     </row>
+    <row r="32" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1580,29 +1610,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17" s="16">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="13"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -1616,41 +1646,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
+      <c r="A21" s="16">
         <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="13"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="13"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="13"/>
+      <c r="C24" s="16"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="13"/>
+      <c r="C25" s="16"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2">

</xml_diff>